<commit_message>
changes on existing scenarios and adding secdep collection sheet scenarios
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/4723-CREATEGROUPW2CLIENTS-SUBMIT(WITHLOCKPRD2MONTHS)01JAN2015-ACTIVATE01JAN2015-DEPOSIT500on15JAN2015-WITHDRAW50on01FEB2015.xlsx
+++ b/Finflux Automation Excels/Client/4723-CREATEGROUPW2CLIENTS-SUBMIT(WITHLOCKPRD2MONTHS)01JAN2015-ACTIVATE01JAN2015-DEPOSIT500on15JAN2015-WITHDRAW50on01FEB2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -162,10 +162,10 @@
     <t>error</t>
   </si>
   <si>
-    <t>Withdrawals blocked until after `01 March 2015`.</t>
-  </si>
-  <si>
     <t>submitteddateon</t>
+  </si>
+  <si>
+    <t>Withdrawals blocked until `01 March 2015`.</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -866,7 +866,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8">
         <v>42005</v>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>